<commit_message>
Break external link in file
</commit_message>
<xml_diff>
--- a/InputData/indst/CtIEPpUESoS/Cost to Impl Eff Policy per Unit E Saved or Shifted.xlsx
+++ b/InputData/indst/CtIEPpUESoS/Cost to Impl Eff Policy per Unit E Saved or Shifted.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-india\InputData\indst\CtIEPpUESoS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-india\InputData\indst\CtIEPpUESoS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,9 +19,6 @@
     <sheet name="India cost adjustment" sheetId="7" r:id="rId5"/>
     <sheet name="CtIEPpUESoS" sheetId="3" r:id="rId6"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId7"/>
-  </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -910,79 +907,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Cover"/>
-      <sheetName val="Summary"/>
-      <sheetName val="Electricity Decarbonization"/>
-      <sheetName val="Industry Elec. - Boilers"/>
-      <sheetName val="Industry Elec. - Process Heat"/>
-      <sheetName val="Industry CCS - Process Heat"/>
-      <sheetName val="Industry Hydrogen &amp; SNG"/>
-      <sheetName val="MDV &amp; HDV Decarbonization"/>
-      <sheetName val="DAC &amp; BECCS"/>
-      <sheetName val="Fuel Costs - PATHWAYS"/>
-      <sheetName val="Emission Factors - PATHWAYS"/>
-      <sheetName val="Constants"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9">
-        <row r="19">
-          <cell r="E19">
-            <v>5.6539999999999999</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="10">
-        <row r="7">
-          <cell r="E7">
-            <v>1.7765038912431299</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="E19">
-            <v>50.07</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="11">
-        <row r="5">
-          <cell r="D5">
-            <v>1055.06</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="D6">
-            <v>3600000</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="C27">
-            <v>229.59399999999999</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="C33">
-            <v>251.107</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2033,7 +1957,6 @@
         <v>105</v>
       </c>
       <c r="C10" s="33">
-        <f>'[1]Fuel Costs - PATHWAYS'!$E$19*([1]Constants!$C$33/[1]Constants!$C$27)*[1]Constants!$D$5/1000</f>
         <v>6.5242598122280206</v>
       </c>
       <c r="D10" s="38"/>
@@ -2046,7 +1969,6 @@
         <v>118</v>
       </c>
       <c r="C11" s="39">
-        <f>'[1]Emission Factors - PATHWAYS'!$E$7/10^9*[1]Constants!$D$6</f>
         <v>6.3954140084752677E-3</v>
       </c>
     </row>
@@ -2058,7 +1980,6 @@
         <v>120</v>
       </c>
       <c r="C12" s="39">
-        <f>'[1]Emission Factors - PATHWAYS'!$E$19*([1]Constants!$D$5/1000)</f>
         <v>52.826854199999993</v>
       </c>
     </row>
@@ -2231,7 +2152,6 @@
         <v>105</v>
       </c>
       <c r="C33" s="33">
-        <f>'[1]Fuel Costs - PATHWAYS'!$E$19*([1]Constants!$C$33/[1]Constants!$C$27)*[1]Constants!$D$5/1000</f>
         <v>6.5242598122280206</v>
       </c>
       <c r="D33" s="25"/>

</xml_diff>